<commit_message>
updated query test -- no significant change, but the rates are listed correctly now.
</commit_message>
<xml_diff>
--- a/discussion/testQuery.xlsx
+++ b/discussion/testQuery.xlsx
@@ -9,23 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="5450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="5450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="S50Q1000" sheetId="8" r:id="rId1"/>
-    <sheet name="S50Q1" sheetId="10" r:id="rId2"/>
-    <sheet name="S1Q1000" sheetId="15" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="11" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="12" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="13" r:id="rId6"/>
-    <sheet name="Sheet4" sheetId="14" r:id="rId7"/>
+    <sheet name="S50Q1000 (2)" sheetId="16" r:id="rId2"/>
+    <sheet name="S50Q1" sheetId="10" r:id="rId3"/>
+    <sheet name="S1Q1000" sheetId="15" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="12" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="13" r:id="rId7"/>
+    <sheet name="Sheet4" sheetId="14" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="109">
   <si>
     <t>N</t>
   </si>
@@ -346,6 +347,12 @@
   </si>
   <si>
     <t>(len 50 factor 10)</t>
+  </si>
+  <si>
+    <t>16 Aug 2019 02:46:50 GMT</t>
+  </si>
+  <si>
+    <t>After final optimization</t>
   </si>
 </sst>
 </file>
@@ -2213,6 +2220,1295 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>100,000-query (width 1000)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> time/ms vs. log N</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'S50Q1000 (2)'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>timeIntNC(len 50 factor 10)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'S50Q1000 (2)'!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.3332456989619628</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6666115684190301</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.3333263404034543</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.6666583547893312</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.3333323879079773</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.6666658401408645</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'S50Q1000 (2)'!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>166.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>166.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>181.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>185.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>198.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>296.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>331.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>376.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A9C3-4553-98D7-8856A9191B6F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'S50Q1000 (2)'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>timeNCList (len 50, factor 10)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'S50Q1000 (2)'!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.3332456989619628</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6666115684190301</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.3333263404034543</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.6666583547893312</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.3333323879079773</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.6666658401408645</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'S50Q1000 (2)'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>237.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>278.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>336.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>374.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>422.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>463.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>480.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A9C3-4553-98D7-8856A9191B6F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'S50Q1000 (2)'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>timeIntLink (len 50, factor 10)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'S50Q1000 (2)'!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.3332456989619628</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6666115684190301</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.3333263404034543</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.6666583547893312</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.3333323879079773</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.6666658401408645</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'S50Q1000 (2)'!$H$2:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>108.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>109.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>136.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>165.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>196.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>243.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A9C3-4553-98D7-8856A9191B6F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="422657936"/>
+        <c:axId val="422653016"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="422657936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="6"/>
+          <c:min val="3"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="422653016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="422653016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="422657936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>100,000-query</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (width 1000) time/ms vs. N</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'S50Q1000 (2)'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>timeIntNC(len 50 factor 10)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'S50Q1000 (2)'!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2154</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4641</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21544</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46415</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>215443</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>464158</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'S50Q1000 (2)'!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>166.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>166.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>181.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>185.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>198.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>296.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>331.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>376.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4CA2-4BF9-9DBA-7101AE23443E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'S50Q1000 (2)'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>timeNCList (len 50, factor 10)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'S50Q1000 (2)'!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2154</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4641</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21544</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46415</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>215443</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>464158</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'S50Q1000 (2)'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>237.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>278.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>336.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>374.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>422.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>463.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>480.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4CA2-4BF9-9DBA-7101AE23443E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'S50Q1000 (2)'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>timeIntLink (len 50, factor 10)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'S50Q1000 (2)'!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2154</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4641</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21544</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46415</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>215443</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>464158</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'S50Q1000 (2)'!$H$2:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>108.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>109.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>136.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>165.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>196.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>243.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4CA2-4BF9-9DBA-7101AE23443E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="422657936"/>
+        <c:axId val="422653016"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="422657936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1000000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="422653016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="422653016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="422657936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>100,000-query (width 1)</a:t>
             </a:r>
             <a:r>
@@ -2802,7 +4098,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3425,7 +4721,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4049,7 +5345,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4912,6 +6208,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -7493,6 +8869,1038 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8079,6 +10487,75 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>307975</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>136525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>3175</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>117475</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>60325</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -8144,7 +10621,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8478,8 +10955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H10"/>
+    <sheetView topLeftCell="A3" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8516,11 +10993,11 @@
         <v>2154</v>
       </c>
       <c r="F2">
-        <f>D19</f>
+        <f t="shared" ref="F2:F8" si="0">D19</f>
         <v>160.4</v>
       </c>
       <c r="G2">
-        <f>D63</f>
+        <f t="shared" ref="G2:G8" si="1">D63</f>
         <v>222.9</v>
       </c>
       <c r="H2">
@@ -8530,22 +11007,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D3">
-        <f t="shared" ref="D3:D6" si="0">LOG10(E3)</f>
+        <f t="shared" ref="D3:D6" si="2">LOG10(E3)</f>
         <v>3.6666115684190301</v>
       </c>
       <c r="E3">
         <v>4641</v>
       </c>
       <c r="F3">
-        <f>D20</f>
+        <f t="shared" si="0"/>
         <v>165.1</v>
       </c>
       <c r="G3">
-        <f>D64</f>
+        <f t="shared" si="1"/>
         <v>232.8</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H10" si="1">D42</f>
+        <f t="shared" ref="H3:H10" si="3">D42</f>
         <v>90.6</v>
       </c>
     </row>
@@ -8558,141 +11035,141 @@
         <v>10000</v>
       </c>
       <c r="F4">
-        <f>D21</f>
+        <f t="shared" si="0"/>
         <v>173.5</v>
       </c>
       <c r="G4">
-        <f>D65</f>
+        <f t="shared" si="1"/>
         <v>241.8</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>95.4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.3333263404034543</v>
       </c>
       <c r="E5">
         <v>21544</v>
       </c>
       <c r="F5">
-        <f>D22</f>
+        <f t="shared" si="0"/>
         <v>183.9</v>
       </c>
       <c r="G5">
-        <f>D66</f>
+        <f t="shared" si="1"/>
         <v>262.60000000000002</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>99.4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.6666583547893312</v>
       </c>
       <c r="E6">
         <v>46415</v>
       </c>
       <c r="F6">
-        <f>D23</f>
+        <f t="shared" si="0"/>
         <v>201.2</v>
       </c>
       <c r="G6">
-        <f>D67</f>
+        <f t="shared" si="1"/>
         <v>306.89999999999998</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>105.7</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D7">
-        <f t="shared" ref="D7:D9" si="2">LOG10(E7)</f>
+        <f t="shared" ref="D7:D9" si="4">LOG10(E7)</f>
         <v>5</v>
       </c>
       <c r="E7">
         <v>100000</v>
       </c>
       <c r="F7">
-        <f>D24</f>
+        <f t="shared" si="0"/>
         <v>244.8</v>
       </c>
       <c r="G7">
-        <f>D68</f>
+        <f t="shared" si="1"/>
         <v>365.3</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>121.5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.3333323879079773</v>
       </c>
       <c r="E8">
         <v>215443</v>
       </c>
       <c r="F8">
-        <f>D25</f>
+        <f t="shared" si="0"/>
         <v>289.7</v>
       </c>
       <c r="G8">
-        <f>D69</f>
+        <f t="shared" si="1"/>
         <v>406.5</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>144.30000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.6666658401408645</v>
       </c>
       <c r="E9">
         <v>464158</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9:F10" si="3">D26</f>
+        <f t="shared" ref="F9:F10" si="5">D26</f>
         <v>327.3</v>
       </c>
       <c r="G9">
-        <f t="shared" ref="G9:G10" si="4">D70</f>
+        <f t="shared" ref="G9:G10" si="6">D70</f>
         <v>435.1</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>169.6</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D10">
-        <f t="shared" ref="D10" si="5">LOG10(E10)</f>
+        <f t="shared" ref="D10" si="7">LOG10(E10)</f>
         <v>6</v>
       </c>
       <c r="E10">
         <v>1000000</v>
       </c>
       <c r="F10">
+        <f t="shared" si="5"/>
+        <v>363.7</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="6"/>
+        <v>467.8</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="3"/>
-        <v>363.7</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="4"/>
-        <v>467.8</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="1"/>
         <v>189.1</v>
       </c>
     </row>
@@ -10118,6 +12595,1339 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <f>LOG10(E2)</f>
+        <v>3.3332456989619628</v>
+      </c>
+      <c r="E2">
+        <v>2154</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F10" si="0">D19</f>
+        <v>166.7</v>
+      </c>
+      <c r="G2">
+        <f>D41</f>
+        <v>237.7</v>
+      </c>
+      <c r="H2">
+        <f>D30</f>
+        <v>108.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <f t="shared" ref="D3:D10" si="1">LOG10(E3)</f>
+        <v>3.6666115684190301</v>
+      </c>
+      <c r="E3">
+        <v>4641</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>166.6</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G10" si="2">D42</f>
+        <v>252</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H10" si="3">D31</f>
+        <v>90.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4">
+        <f>LOG10(E4)</f>
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>10000</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>181.2</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>251</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>4.3333263404034543</v>
+      </c>
+      <c r="E5">
+        <v>21544</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>185.2</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>278.7</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>4.6666583547893312</v>
+      </c>
+      <c r="E6">
+        <v>46415</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>198.4</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>336.8</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>109.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>100000</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>254</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>374.7</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>136.69999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>5.3333323879079773</v>
+      </c>
+      <c r="E8">
+        <v>215443</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>296.60000000000002</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>422.1</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>165.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>5.6666658401408645</v>
+      </c>
+      <c r="E9">
+        <v>464158</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>331.9</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>463.7</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>196.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>1000000</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>376.6</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>480.5</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>243.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>2154</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>166.7</v>
+      </c>
+      <c r="E19">
+        <v>601.79999999999995</v>
+      </c>
+      <c r="F19">
+        <v>3.29</v>
+      </c>
+      <c r="G19">
+        <v>11.64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>4641</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>166.6</v>
+      </c>
+      <c r="E20">
+        <v>600.5</v>
+      </c>
+      <c r="F20">
+        <v>1.46</v>
+      </c>
+      <c r="G20">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>10000</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>181.2</v>
+      </c>
+      <c r="E21">
+        <v>553.20000000000005</v>
+      </c>
+      <c r="F21">
+        <v>3.02</v>
+      </c>
+      <c r="G21">
+        <v>8.76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>21544</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>185.2</v>
+      </c>
+      <c r="E22">
+        <v>541.4</v>
+      </c>
+      <c r="F22">
+        <v>3.5</v>
+      </c>
+      <c r="G22">
+        <v>9.2200000000000006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>46415</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>198.4</v>
+      </c>
+      <c r="E23">
+        <v>504.2</v>
+      </c>
+      <c r="F23">
+        <v>0.95</v>
+      </c>
+      <c r="G23">
+        <v>2.39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>100000</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>254</v>
+      </c>
+      <c r="E24">
+        <v>396.3</v>
+      </c>
+      <c r="F24">
+        <v>7.34</v>
+      </c>
+      <c r="G24">
+        <v>10.119999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>215443</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>296.60000000000002</v>
+      </c>
+      <c r="E25">
+        <v>338.2</v>
+      </c>
+      <c r="F25">
+        <v>5.8</v>
+      </c>
+      <c r="G25">
+        <v>5.87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>464158</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>331.9</v>
+      </c>
+      <c r="E26">
+        <v>301.39999999999998</v>
+      </c>
+      <c r="F26">
+        <v>2.52</v>
+      </c>
+      <c r="G26">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <v>1000000</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>376.6</v>
+      </c>
+      <c r="E27">
+        <v>266.2</v>
+      </c>
+      <c r="F27">
+        <v>6.6</v>
+      </c>
+      <c r="G27">
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>2154</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>108.3</v>
+      </c>
+      <c r="E30">
+        <v>929.5</v>
+      </c>
+      <c r="F30">
+        <v>3.16</v>
+      </c>
+      <c r="G30">
+        <v>24.14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31">
+        <v>4641</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>90.8</v>
+      </c>
+      <c r="E31">
+        <v>1102</v>
+      </c>
+      <c r="F31">
+        <v>0.27</v>
+      </c>
+      <c r="G31">
+        <v>3.24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32">
+        <v>10000</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>98</v>
+      </c>
+      <c r="E32">
+        <v>1022.3</v>
+      </c>
+      <c r="F32">
+        <v>1.35</v>
+      </c>
+      <c r="G32">
+        <v>12.89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>21544</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>103</v>
+      </c>
+      <c r="E33">
+        <v>971</v>
+      </c>
+      <c r="F33">
+        <v>0.39</v>
+      </c>
+      <c r="G33">
+        <v>3.67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>46415</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>109.4</v>
+      </c>
+      <c r="E34">
+        <v>914.4</v>
+      </c>
+      <c r="F34">
+        <v>0.45</v>
+      </c>
+      <c r="G34">
+        <v>3.78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35">
+        <v>100000</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>136.69999999999999</v>
+      </c>
+      <c r="E35">
+        <v>739.8</v>
+      </c>
+      <c r="F35">
+        <v>5.09</v>
+      </c>
+      <c r="G35">
+        <v>24.09</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36">
+        <v>215443</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <v>165.7</v>
+      </c>
+      <c r="E36">
+        <v>605.9</v>
+      </c>
+      <c r="F36">
+        <v>3.68</v>
+      </c>
+      <c r="G36">
+        <v>11.98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37">
+        <v>464158</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+      <c r="D37">
+        <v>196.8</v>
+      </c>
+      <c r="E37">
+        <v>509.6</v>
+      </c>
+      <c r="F37">
+        <v>3.86</v>
+      </c>
+      <c r="G37">
+        <v>8.66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38">
+        <v>1000000</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <v>243.6</v>
+      </c>
+      <c r="E38">
+        <v>414.4</v>
+      </c>
+      <c r="F38">
+        <v>8.23</v>
+      </c>
+      <c r="G38">
+        <v>12.49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>2154</v>
+      </c>
+      <c r="C41">
+        <v>10</v>
+      </c>
+      <c r="D41">
+        <v>237.7</v>
+      </c>
+      <c r="E41">
+        <v>421.1</v>
+      </c>
+      <c r="F41">
+        <v>2.08</v>
+      </c>
+      <c r="G41">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>4641</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <v>252</v>
+      </c>
+      <c r="E42">
+        <v>398.2</v>
+      </c>
+      <c r="F42">
+        <v>5.13</v>
+      </c>
+      <c r="G42">
+        <v>7.58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>10000</v>
+      </c>
+      <c r="C43">
+        <v>10</v>
+      </c>
+      <c r="D43">
+        <v>251</v>
+      </c>
+      <c r="E43">
+        <v>399.7</v>
+      </c>
+      <c r="F43">
+        <v>4.82</v>
+      </c>
+      <c r="G43">
+        <v>7.05</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>21544</v>
+      </c>
+      <c r="C44">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>278.7</v>
+      </c>
+      <c r="E44">
+        <v>360.2</v>
+      </c>
+      <c r="F44">
+        <v>5.92</v>
+      </c>
+      <c r="G44">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>46415</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
+      </c>
+      <c r="D45">
+        <v>336.8</v>
+      </c>
+      <c r="E45">
+        <v>297.39999999999998</v>
+      </c>
+      <c r="F45">
+        <v>4.57</v>
+      </c>
+      <c r="G45">
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46">
+        <v>100000</v>
+      </c>
+      <c r="C46">
+        <v>10</v>
+      </c>
+      <c r="D46">
+        <v>374.7</v>
+      </c>
+      <c r="E46">
+        <v>267</v>
+      </c>
+      <c r="F46">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G46">
+        <v>1.63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <v>215443</v>
+      </c>
+      <c r="C47">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>422.1</v>
+      </c>
+      <c r="E47">
+        <v>237.3</v>
+      </c>
+      <c r="F47">
+        <v>6.09</v>
+      </c>
+      <c r="G47">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>464158</v>
+      </c>
+      <c r="C48">
+        <v>10</v>
+      </c>
+      <c r="D48">
+        <v>463.7</v>
+      </c>
+      <c r="E48">
+        <v>216.2</v>
+      </c>
+      <c r="F48">
+        <v>8.26</v>
+      </c>
+      <c r="G48">
+        <v>3.64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>1000000</v>
+      </c>
+      <c r="C49">
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <v>480.5</v>
+      </c>
+      <c r="E49">
+        <v>208.6</v>
+      </c>
+      <c r="F49">
+        <v>8.27</v>
+      </c>
+      <c r="G49">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70">
+        <v>464158</v>
+      </c>
+      <c r="C70">
+        <v>10</v>
+      </c>
+      <c r="D70">
+        <v>435.1</v>
+      </c>
+      <c r="E70">
+        <v>1066.9000000000001</v>
+      </c>
+      <c r="F70">
+        <v>0.21</v>
+      </c>
+      <c r="G70">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71">
+        <v>1000000</v>
+      </c>
+      <c r="C71">
+        <v>10</v>
+      </c>
+      <c r="D71">
+        <v>467.8</v>
+      </c>
+      <c r="E71">
+        <v>2142.6999999999998</v>
+      </c>
+      <c r="F71">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="G71">
+        <v>32.380000000000003</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>41</v>
+      </c>
+      <c r="B74">
+        <v>2154</v>
+      </c>
+      <c r="C74">
+        <v>10</v>
+      </c>
+      <c r="D74">
+        <v>230.3</v>
+      </c>
+      <c r="E74">
+        <v>9.4</v>
+      </c>
+      <c r="F74">
+        <v>2.1</v>
+      </c>
+      <c r="G74">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>41</v>
+      </c>
+      <c r="B75">
+        <v>4641</v>
+      </c>
+      <c r="C75">
+        <v>10</v>
+      </c>
+      <c r="D75">
+        <v>239.7</v>
+      </c>
+      <c r="E75">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="F75">
+        <v>0.86</v>
+      </c>
+      <c r="G75">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>41</v>
+      </c>
+      <c r="B76">
+        <v>10000</v>
+      </c>
+      <c r="C76">
+        <v>10</v>
+      </c>
+      <c r="D76">
+        <v>246.3</v>
+      </c>
+      <c r="E76">
+        <v>40.6</v>
+      </c>
+      <c r="F76">
+        <v>0.27</v>
+      </c>
+      <c r="G76">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>41</v>
+      </c>
+      <c r="B77">
+        <v>21544</v>
+      </c>
+      <c r="C77">
+        <v>10</v>
+      </c>
+      <c r="D77">
+        <v>260.3</v>
+      </c>
+      <c r="E77">
+        <v>82.8</v>
+      </c>
+      <c r="F77">
+        <v>0.85</v>
+      </c>
+      <c r="G77">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>41</v>
+      </c>
+      <c r="B78">
+        <v>46415</v>
+      </c>
+      <c r="C78">
+        <v>10</v>
+      </c>
+      <c r="D78">
+        <v>310.2</v>
+      </c>
+      <c r="E78">
+        <v>149.6</v>
+      </c>
+      <c r="F78">
+        <v>0.37</v>
+      </c>
+      <c r="G78">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>41</v>
+      </c>
+      <c r="B79">
+        <v>100000</v>
+      </c>
+      <c r="C79">
+        <v>10</v>
+      </c>
+      <c r="D79">
+        <v>365</v>
+      </c>
+      <c r="E79">
+        <v>274</v>
+      </c>
+      <c r="F79">
+        <v>0.64</v>
+      </c>
+      <c r="G79">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>41</v>
+      </c>
+      <c r="B80">
+        <v>215443</v>
+      </c>
+      <c r="C80">
+        <v>10</v>
+      </c>
+      <c r="D80">
+        <v>404.9</v>
+      </c>
+      <c r="E80">
+        <v>532.1</v>
+      </c>
+      <c r="F80">
+        <v>0.33</v>
+      </c>
+      <c r="G80">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>41</v>
+      </c>
+      <c r="B81">
+        <v>464158</v>
+      </c>
+      <c r="C81">
+        <v>10</v>
+      </c>
+      <c r="D81">
+        <v>434.4</v>
+      </c>
+      <c r="E81">
+        <v>1068.5999999999999</v>
+      </c>
+      <c r="F81">
+        <v>0.66</v>
+      </c>
+      <c r="G81">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>41</v>
+      </c>
+      <c r="B82">
+        <v>1000000</v>
+      </c>
+      <c r="C82">
+        <v>10</v>
+      </c>
+      <c r="D82">
+        <v>462.4</v>
+      </c>
+      <c r="E82">
+        <v>2163.4</v>
+      </c>
+      <c r="F82">
+        <v>3.36</v>
+      </c>
+      <c r="G82">
+        <v>14.88</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H100"/>
   <sheetViews>
@@ -11733,7 +15543,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I100"/>
   <sheetViews>
@@ -13358,7 +17168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
@@ -13690,7 +17500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
@@ -14022,7 +17832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
@@ -14354,7 +18164,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>

</xml_diff>